<commit_message>
Finished half the graphs
</commit_message>
<xml_diff>
--- a/Assessment 2 v1/Results Waypoint 1.xlsx
+++ b/Assessment 2 v1/Results Waypoint 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/kk19332_bristol_ac_uk/Documents/Documents/Eng Des/Year 5/Robotics-Systems-A2/Assessment 2 v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{7C8E6764-BAA2-4701-82AB-F97D09BB8F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F51F70C0-ED12-4D31-8C11-2FB388EB75D1}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{7C8E6764-BAA2-4701-82AB-F97D09BB8F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C56DA805-6A2B-4B8C-AC00-CB1333E7BD9A}"/>
   <bookViews>
-    <workbookView xWindow="6429" yWindow="214" windowWidth="19285" windowHeight="12026" xr2:uid="{506BA83C-A7B3-43C5-AD2D-E0CAB2B7B6B9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{506BA83C-A7B3-43C5-AD2D-E0CAB2B7B6B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Waypoints" sheetId="1" r:id="rId1"/>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5BCB56-9515-413D-9030-3E612E14AC95}">
   <dimension ref="A1:EZ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EJ1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="EV17" sqref="EV17"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="CM21" sqref="CM21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>